<commit_message>
Updated with Code Changes
</commit_message>
<xml_diff>
--- a/Case Study 2/Significant Table.xlsx
+++ b/Case Study 2/Significant Table.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="14_{CA3B5123-ED1E-5440-8546-D5D82B1A5E4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="3060" windowWidth="30420" windowHeight="18240" activeTab="1" xr2:uid="{27BABDC8-95E6-4834-B961-269F4E578523}"/>
+    <workbookView xWindow="260" yWindow="3060" windowWidth="30420" windowHeight="18240" activeTab="1" xr2:uid="{27BABDC8-95E6-4834-B961-269F4E578523}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -2380,7 +2380,7 @@
   <dimension ref="A1:AW20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B5" sqref="B5:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>